<commit_message>
Minor modifications to some documentation; started schematic.
</commit_message>
<xml_diff>
--- a/Documentation/cyclone-iii-pinout.xlsx
+++ b/Documentation/cyclone-iii-pinout.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="273">
   <si>
     <t>Pin</t>
   </si>
@@ -678,9 +678,6 @@
     <t>i2c CS</t>
   </si>
   <si>
-    <t>Switch Debounce CS</t>
-  </si>
-  <si>
     <t>Rotary Switch CS</t>
   </si>
   <si>
@@ -699,9 +696,6 @@
     <t>Enable Data from Rotary Switches</t>
   </si>
   <si>
-    <t>Enable Data from Switches</t>
-  </si>
-  <si>
     <t>Real-Time Math CS</t>
   </si>
   <si>
@@ -820,6 +814,30 @@
   </si>
   <si>
     <t>Albert Gural</t>
+  </si>
+  <si>
+    <t>ASDI</t>
+  </si>
+  <si>
+    <t>ASDI of Serial Config. Device</t>
+  </si>
+  <si>
+    <t>DCLK of Serial Config. Device</t>
+  </si>
+  <si>
+    <t>nCS</t>
+  </si>
+  <si>
+    <t>nCS of Serial Config. Device</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>DATA of Serial Config. Device</t>
+  </si>
+  <si>
+    <t>Tie High to keep chip on</t>
   </si>
 </sst>
 </file>
@@ -1079,14 +1097,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1391,8 +1409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F185"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,18 +1423,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F1" s="16" t="s">
-        <v>266</v>
+      <c r="F1" s="14" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="14" t="s">
-        <v>265</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="B2" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
@@ -1463,7 +1481,7 @@
         <v>186</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>191</v>
@@ -2109,10 +2127,10 @@
         <v>197</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
@@ -2126,10 +2144,10 @@
         <v>200</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>247</v>
+        <v>205</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>248</v>
+        <v>272</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
@@ -2160,10 +2178,10 @@
         <v>186</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>186</v>
+        <v>270</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>186</v>
+        <v>271</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
@@ -2177,10 +2195,10 @@
         <v>186</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>186</v>
+        <v>267</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
@@ -2197,7 +2215,7 @@
         <v>204</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
@@ -2214,7 +2232,7 @@
         <v>204</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
@@ -2231,7 +2249,7 @@
         <v>204</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
@@ -2316,7 +2334,7 @@
         <v>215</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
@@ -2333,7 +2351,7 @@
         <v>216</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
@@ -2350,7 +2368,7 @@
         <v>217</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
@@ -2367,7 +2385,7 @@
         <v>218</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
@@ -2381,10 +2399,10 @@
         <v>210</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>219</v>
+        <v>265</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
@@ -2415,10 +2433,10 @@
         <v>200</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>186</v>
+        <v>268</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>186</v>
+        <v>269</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
@@ -2432,10 +2450,10 @@
         <v>210</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.25">
@@ -2449,10 +2467,10 @@
         <v>210</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
@@ -2466,10 +2484,10 @@
         <v>210</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
@@ -2483,10 +2501,10 @@
         <v>210</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
@@ -2500,10 +2518,10 @@
         <v>210</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
@@ -2517,10 +2535,10 @@
         <v>210</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.25">
@@ -2534,10 +2552,10 @@
         <v>210</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
@@ -2551,10 +2569,10 @@
         <v>197</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
@@ -2568,10 +2586,10 @@
         <v>197</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
@@ -2585,10 +2603,10 @@
         <v>197</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.25">
@@ -2619,10 +2637,10 @@
         <v>210</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.25">
@@ -2687,10 +2705,10 @@
         <v>197</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.25">
@@ -2704,10 +2722,10 @@
         <v>197</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.25">
@@ -2721,10 +2739,10 @@
         <v>197</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.25">
@@ -2738,10 +2756,10 @@
         <v>197</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.25">
@@ -2755,10 +2773,10 @@
         <v>197</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.25">
@@ -2772,10 +2790,10 @@
         <v>197</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.25">
@@ -2789,10 +2807,10 @@
         <v>197</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.25">
@@ -2840,10 +2858,10 @@
         <v>197</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.25">
@@ -2857,10 +2875,10 @@
         <v>197</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.25">
@@ -2874,10 +2892,10 @@
         <v>197</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.25">
@@ -2908,10 +2926,10 @@
         <v>197</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.25">
@@ -2925,10 +2943,10 @@
         <v>197</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.25">
@@ -2942,10 +2960,10 @@
         <v>197</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.25">
@@ -2959,10 +2977,10 @@
         <v>197</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.25">
@@ -2976,10 +2994,10 @@
         <v>197</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.25">
@@ -2993,10 +3011,10 @@
         <v>197</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.25">
@@ -3010,10 +3028,10 @@
         <v>197</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.25">
@@ -3027,10 +3045,10 @@
         <v>197</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.25">
@@ -3044,10 +3062,10 @@
         <v>197</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.25">
@@ -3061,10 +3079,10 @@
         <v>197</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.25">
@@ -3078,10 +3096,10 @@
         <v>197</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.25">
@@ -3095,10 +3113,10 @@
         <v>197</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.25">
@@ -3112,10 +3130,10 @@
         <v>197</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.25">
@@ -3129,10 +3147,10 @@
         <v>197</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.25">
@@ -3146,10 +3164,10 @@
         <v>197</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.25">
@@ -3163,10 +3181,10 @@
         <v>197</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.25">
@@ -3197,10 +3215,10 @@
         <v>197</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.25">
@@ -3214,10 +3232,10 @@
         <v>197</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.25">
@@ -3231,10 +3249,10 @@
         <v>197</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.25">
@@ -3282,10 +3300,10 @@
         <v>197</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.25">
@@ -3299,10 +3317,10 @@
         <v>197</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.25">
@@ -3350,10 +3368,10 @@
         <v>200</v>
       </c>
       <c r="E116" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F116" s="4" t="s">
         <v>259</v>
-      </c>
-      <c r="F116" s="4" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.25">
@@ -3367,10 +3385,10 @@
         <v>200</v>
       </c>
       <c r="E117" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F117" s="4" t="s">
         <v>260</v>
-      </c>
-      <c r="F117" s="4" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.25">
@@ -3418,10 +3436,10 @@
         <v>197</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.25">
@@ -3537,10 +3555,10 @@
         <v>197</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F127" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.25">
@@ -3554,10 +3572,10 @@
         <v>197</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F128" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.25">
@@ -3622,10 +3640,10 @@
         <v>197</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F132" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="133" spans="2:6" x14ac:dyDescent="0.25">
@@ -3639,10 +3657,10 @@
         <v>197</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F133" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="134" spans="2:6" x14ac:dyDescent="0.25">
@@ -3656,10 +3674,10 @@
         <v>197</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F134" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="135" spans="2:6" x14ac:dyDescent="0.25">
@@ -4200,10 +4218,10 @@
         <v>197</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F166" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="167" spans="2:6" x14ac:dyDescent="0.25">
@@ -4217,10 +4235,10 @@
         <v>197</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F167" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="168" spans="2:6" x14ac:dyDescent="0.25">
@@ -4234,10 +4252,10 @@
         <v>197</v>
       </c>
       <c r="E168" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F168" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="169" spans="2:6" x14ac:dyDescent="0.25">
@@ -4251,10 +4269,10 @@
         <v>197</v>
       </c>
       <c r="E169" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F169" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="170" spans="2:6" x14ac:dyDescent="0.25">
@@ -4268,10 +4286,10 @@
         <v>197</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F170" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="171" spans="2:6" x14ac:dyDescent="0.25">
@@ -4285,10 +4303,10 @@
         <v>197</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F171" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="172" spans="2:6" x14ac:dyDescent="0.25">
@@ -4302,10 +4320,10 @@
         <v>197</v>
       </c>
       <c r="E172" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F172" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="173" spans="2:6" x14ac:dyDescent="0.25">
@@ -4319,10 +4337,10 @@
         <v>197</v>
       </c>
       <c r="E173" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F173" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="174" spans="2:6" x14ac:dyDescent="0.25">
@@ -4336,10 +4354,10 @@
         <v>197</v>
       </c>
       <c r="E174" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F174" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="175" spans="2:6" x14ac:dyDescent="0.25">
@@ -4353,10 +4371,10 @@
         <v>197</v>
       </c>
       <c r="E175" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F175" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="176" spans="2:6" x14ac:dyDescent="0.25">
@@ -4370,10 +4388,10 @@
         <v>197</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F176" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="177" spans="2:6" x14ac:dyDescent="0.25">
@@ -4387,10 +4405,10 @@
         <v>210</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F177" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="178" spans="2:6" x14ac:dyDescent="0.25">
@@ -4404,10 +4422,10 @@
         <v>210</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F178" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="179" spans="2:6" x14ac:dyDescent="0.25">
@@ -4421,10 +4439,10 @@
         <v>210</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F179" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="180" spans="2:6" x14ac:dyDescent="0.25">
@@ -4438,10 +4456,10 @@
         <v>210</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F180" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="181" spans="2:6" x14ac:dyDescent="0.25">
@@ -4455,10 +4473,10 @@
         <v>210</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F181" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="182" spans="2:6" x14ac:dyDescent="0.25">
@@ -4472,10 +4490,10 @@
         <v>210</v>
       </c>
       <c r="E182" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F182" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="183" spans="2:6" x14ac:dyDescent="0.25">
@@ -4489,10 +4507,10 @@
         <v>210</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F183" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="184" spans="2:6" x14ac:dyDescent="0.25">
@@ -4506,10 +4524,10 @@
         <v>210</v>
       </c>
       <c r="E184" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F184" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="185" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4523,10 +4541,10 @@
         <v>210</v>
       </c>
       <c r="E185" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F185" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Began fixing initial schematic; changed I/O designations.
</commit_message>
<xml_diff>
--- a/Documentation/cyclone-iii-pinout.xlsx
+++ b/Documentation/cyclone-iii-pinout.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="294">
   <si>
     <t>Pin</t>
   </si>
@@ -666,45 +666,12 @@
     <t>VRAM CS</t>
   </si>
   <si>
-    <t>i2c CS</t>
-  </si>
-  <si>
-    <t>Rotary Switch CS</t>
-  </si>
-  <si>
     <t>Enable SRAM</t>
   </si>
   <si>
     <t>Enable VRAM</t>
   </si>
   <si>
-    <t>Enable i2c</t>
-  </si>
-  <si>
-    <t>Enable Data from Rotary Switches</t>
-  </si>
-  <si>
-    <t>Enable Data from Switches</t>
-  </si>
-  <si>
-    <t>Real-Time Math CS</t>
-  </si>
-  <si>
-    <t>Enable Data from Real-time Math</t>
-  </si>
-  <si>
-    <t>Input Queues CS</t>
-  </si>
-  <si>
-    <t>Enable Data from Input Queues</t>
-  </si>
-  <si>
-    <t>Compare Regs. CS</t>
-  </si>
-  <si>
-    <t>Enable Data to Compare Registers</t>
-  </si>
-  <si>
     <t>R/W Control</t>
   </si>
   <si>
@@ -717,30 +684,6 @@
     <t>Clears WDT Counter</t>
   </si>
   <si>
-    <t>Switch Int.</t>
-  </si>
-  <si>
-    <t>Indicates switch change</t>
-  </si>
-  <si>
-    <t>Rot. Switch Int.</t>
-  </si>
-  <si>
-    <t>Indicates rotary switch move</t>
-  </si>
-  <si>
-    <t>Queue Full Int.</t>
-  </si>
-  <si>
-    <t>Indicates queue full</t>
-  </si>
-  <si>
-    <t>Trigger Reset</t>
-  </si>
-  <si>
-    <t>Resets trigger circuitry</t>
-  </si>
-  <si>
     <t>Reset Circuitry</t>
   </si>
   <si>
@@ -783,12 +726,6 @@
     <t>i2c SDA</t>
   </si>
   <si>
-    <t>i2c Clock pin</t>
-  </si>
-  <si>
-    <t>i2c Data pin</t>
-  </si>
-  <si>
     <t>Cyclone III (EPC340) Pins</t>
   </si>
   <si>
@@ -834,28 +771,136 @@
     <t>VRAM Col Address Strobe</t>
   </si>
   <si>
-    <t>Output Enable</t>
-  </si>
-  <si>
-    <t>Enables Chip Outputs</t>
-  </si>
-  <si>
-    <t>Switch CS</t>
-  </si>
-  <si>
     <t>Flash CS</t>
   </si>
   <si>
     <t>Data Bus Out</t>
   </si>
   <si>
-    <t>i2c Out</t>
-  </si>
-  <si>
     <t>Use Data Bus as Output</t>
   </si>
   <si>
-    <t>Use i2c as Output</t>
+    <t>ADC Clock Out</t>
+  </si>
+  <si>
+    <t>ADC Clock Output</t>
+  </si>
+  <si>
+    <t>SPI FSYNC</t>
+  </si>
+  <si>
+    <t>SPI MOSI</t>
+  </si>
+  <si>
+    <t>SPI SCK</t>
+  </si>
+  <si>
+    <t>General Port 8</t>
+  </si>
+  <si>
+    <t>User-selectable port 8</t>
+  </si>
+  <si>
+    <t>General Port 9</t>
+  </si>
+  <si>
+    <t>User-selectable port 9</t>
+  </si>
+  <si>
+    <t>General Port 10</t>
+  </si>
+  <si>
+    <t>General Port 11</t>
+  </si>
+  <si>
+    <t>General Port 12</t>
+  </si>
+  <si>
+    <t>General Port 13</t>
+  </si>
+  <si>
+    <t>General Port 14</t>
+  </si>
+  <si>
+    <t>General Port 15</t>
+  </si>
+  <si>
+    <t>General Port H I/O</t>
+  </si>
+  <si>
+    <t>User-selectable high port in/out</t>
+  </si>
+  <si>
+    <t>General Port L I/O</t>
+  </si>
+  <si>
+    <t>User-selectable low port in/out</t>
+  </si>
+  <si>
+    <t>General Port 0</t>
+  </si>
+  <si>
+    <t>General Port 1</t>
+  </si>
+  <si>
+    <t>General Port 2</t>
+  </si>
+  <si>
+    <t>General Port 3</t>
+  </si>
+  <si>
+    <t>General Port 4</t>
+  </si>
+  <si>
+    <t>General Port 5</t>
+  </si>
+  <si>
+    <t>General Port 6</t>
+  </si>
+  <si>
+    <t>General Port 7</t>
+  </si>
+  <si>
+    <t>User-selectable port 7</t>
+  </si>
+  <si>
+    <t>User-selectable port 6</t>
+  </si>
+  <si>
+    <t>User-selectable port 5</t>
+  </si>
+  <si>
+    <t>User-selectable port 4</t>
+  </si>
+  <si>
+    <t>User-selectable port 3</t>
+  </si>
+  <si>
+    <t>User-selectable port 2</t>
+  </si>
+  <si>
+    <t>User-selectable port 1</t>
+  </si>
+  <si>
+    <t>User-selectable port 0</t>
+  </si>
+  <si>
+    <t>User-selectable port 15</t>
+  </si>
+  <si>
+    <t>User-selectable port 14</t>
+  </si>
+  <si>
+    <t>User-selectable port 13</t>
+  </si>
+  <si>
+    <t>User-selectable port 12</t>
+  </si>
+  <si>
+    <t>User-selectable port 11</t>
+  </si>
+  <si>
+    <t>User-selectable port 10</t>
   </si>
 </sst>
 </file>
@@ -1169,12 +1214,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1186,6 +1225,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1494,8 +1539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F185"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F178" sqref="F178"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H168" sqref="H168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,17 +1554,17 @@
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F1" s="11" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+      <c r="B2" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
@@ -1539,19 +1584,19 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="E4" s="23" t="s">
+      <c r="C4" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="E4" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="22" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2212,10 +2257,10 @@
         <v>196</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
@@ -2232,7 +2277,7 @@
         <v>204</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
@@ -2263,10 +2308,10 @@
         <v>185</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
@@ -2283,7 +2328,7 @@
         <v>48</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
@@ -2300,7 +2345,7 @@
         <v>203</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2317,7 +2362,7 @@
         <v>203</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2334,7 +2379,7 @@
         <v>203</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2406,7 +2451,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="14"/>
+      <c r="A55" s="12"/>
       <c r="B55" s="3" t="s">
         <v>56</v>
       </c>
@@ -2417,14 +2462,14 @@
         <v>209</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="14"/>
+      <c r="A56" s="12"/>
       <c r="B56" s="3" t="s">
         <v>57</v>
       </c>
@@ -2438,11 +2483,11 @@
         <v>213</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
+      <c r="A57" s="12"/>
       <c r="B57" s="3" t="s">
         <v>58</v>
       </c>
@@ -2456,11 +2501,11 @@
         <v>214</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
+      <c r="A58" s="12"/>
       <c r="B58" s="3" t="s">
         <v>59</v>
       </c>
@@ -2471,14 +2516,14 @@
         <v>209</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
+      <c r="A59" s="12"/>
       <c r="B59" s="3" t="s">
         <v>60</v>
       </c>
@@ -2489,14 +2534,14 @@
         <v>209</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>258</v>
+        <v>237</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
+      <c r="A60" s="12"/>
       <c r="B60" s="3" t="s">
         <v>61</v>
       </c>
@@ -2507,14 +2552,14 @@
         <v>209</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
+      <c r="A61" s="12"/>
       <c r="B61" s="3" t="s">
         <v>62</v>
       </c>
@@ -2525,32 +2570,32 @@
         <v>199</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
+      <c r="A62" s="12"/>
       <c r="B62" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>209</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
+      <c r="A63" s="12"/>
       <c r="B63" s="3" t="s">
         <v>64</v>
       </c>
@@ -2561,86 +2606,86 @@
         <v>209</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>273</v>
+        <v>219</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
+      <c r="A64" s="12"/>
       <c r="B64" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>216</v>
+        <v>185</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>220</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="15"/>
+      <c r="A65" s="13"/>
       <c r="B65" s="3" t="s">
         <v>66</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
+      <c r="A66" s="13"/>
       <c r="B66" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="15"/>
+      <c r="A67" s="13"/>
       <c r="B67" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="15"/>
+      <c r="A68" s="13"/>
       <c r="B68" s="3" t="s">
         <v>69</v>
       </c>
@@ -2648,17 +2693,17 @@
         <v>200</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>271</v>
+        <v>231</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>272</v>
+        <v>232</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="15"/>
+      <c r="A69" s="13"/>
       <c r="B69" s="3" t="s">
         <v>70</v>
       </c>
@@ -2666,53 +2711,53 @@
         <v>200</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
+      <c r="A70" s="13"/>
       <c r="B70" s="3" t="s">
         <v>71</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="15"/>
+      <c r="A71" s="13"/>
       <c r="B71" s="3" t="s">
         <v>71</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="15"/>
+      <c r="A72" s="13"/>
       <c r="B72" s="3" t="s">
         <v>72</v>
       </c>
@@ -2723,14 +2768,14 @@
         <v>196</v>
       </c>
       <c r="E72" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F72" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="F72" s="4" t="s">
-        <v>233</v>
-      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="15"/>
+      <c r="A73" s="13"/>
       <c r="B73" s="3" t="s">
         <v>73</v>
       </c>
@@ -2741,14 +2786,14 @@
         <v>196</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="15"/>
+      <c r="A74" s="13"/>
       <c r="B74" s="3" t="s">
         <v>74</v>
       </c>
@@ -2759,104 +2804,104 @@
         <v>196</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="15"/>
+      <c r="A75" s="13"/>
       <c r="B75" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>185</v>
+        <v>233</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>185</v>
+        <v>233</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="15"/>
+      <c r="A76" s="13"/>
       <c r="B76" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>185</v>
+        <v>234</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>185</v>
+        <v>234</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="15"/>
+      <c r="A77" s="13"/>
       <c r="B77" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>185</v>
+        <v>255</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>185</v>
+        <v>255</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="15"/>
+      <c r="A78" s="13"/>
       <c r="B78" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>185</v>
+        <v>256</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>185</v>
+        <v>256</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="15"/>
+      <c r="A79" s="13"/>
       <c r="B79" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>185</v>
+        <v>257</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>185</v>
+        <v>257</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="16"/>
+      <c r="A80" s="14"/>
       <c r="B80" s="3" t="s">
         <v>80</v>
       </c>
@@ -2867,14 +2912,14 @@
         <v>196</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="16"/>
+      <c r="A81" s="14"/>
       <c r="B81" s="3" t="s">
         <v>81</v>
       </c>
@@ -2885,14 +2930,14 @@
         <v>196</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="16"/>
+      <c r="A82" s="14"/>
       <c r="B82" s="3" t="s">
         <v>82</v>
       </c>
@@ -2903,14 +2948,14 @@
         <v>196</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="16"/>
+      <c r="A83" s="14"/>
       <c r="B83" s="3" t="s">
         <v>83</v>
       </c>
@@ -2921,32 +2966,32 @@
         <v>196</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="16"/>
+      <c r="A84" s="14"/>
       <c r="B84" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>185</v>
+        <v>253</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>185</v>
+        <v>254</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="16"/>
+      <c r="A85" s="14"/>
       <c r="B85" s="3" t="s">
         <v>85</v>
       </c>
@@ -2964,7 +3009,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="16"/>
+      <c r="A86" s="14"/>
       <c r="B86" s="3" t="s">
         <v>86</v>
       </c>
@@ -2975,14 +3020,14 @@
         <v>196</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="16"/>
+      <c r="A87" s="14"/>
       <c r="B87" s="3" t="s">
         <v>87</v>
       </c>
@@ -2993,14 +3038,14 @@
         <v>196</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="16"/>
+      <c r="A88" s="14"/>
       <c r="B88" s="3" t="s">
         <v>88</v>
       </c>
@@ -3011,14 +3056,14 @@
         <v>196</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="16"/>
+      <c r="A89" s="14"/>
       <c r="B89" s="3" t="s">
         <v>89</v>
       </c>
@@ -3029,14 +3074,14 @@
         <v>196</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="16"/>
+      <c r="A90" s="14"/>
       <c r="B90" s="3" t="s">
         <v>90</v>
       </c>
@@ -3047,14 +3092,14 @@
         <v>196</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="16"/>
+      <c r="A91" s="14"/>
       <c r="B91" s="3" t="s">
         <v>91</v>
       </c>
@@ -3065,14 +3110,14 @@
         <v>196</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="16"/>
+      <c r="A92" s="14"/>
       <c r="B92" s="3" t="s">
         <v>92</v>
       </c>
@@ -3083,14 +3128,14 @@
         <v>196</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="16"/>
+      <c r="A93" s="14"/>
       <c r="B93" s="3" t="s">
         <v>93</v>
       </c>
@@ -3101,14 +3146,14 @@
         <v>196</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="16"/>
+      <c r="A94" s="14"/>
       <c r="B94" s="3" t="s">
         <v>94</v>
       </c>
@@ -3119,14 +3164,14 @@
         <v>196</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="16"/>
+      <c r="A95" s="14"/>
       <c r="B95" s="3" t="s">
         <v>95</v>
       </c>
@@ -3137,14 +3182,14 @@
         <v>196</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="16"/>
+      <c r="A96" s="14"/>
       <c r="B96" s="3" t="s">
         <v>96</v>
       </c>
@@ -3155,14 +3200,14 @@
         <v>196</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="16"/>
+      <c r="A97" s="14"/>
       <c r="B97" s="3" t="s">
         <v>97</v>
       </c>
@@ -3173,14 +3218,14 @@
         <v>196</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="17"/>
+      <c r="A98" s="15"/>
       <c r="B98" s="3" t="s">
         <v>98</v>
       </c>
@@ -3198,7 +3243,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="17"/>
+      <c r="A99" s="15"/>
       <c r="B99" s="3" t="s">
         <v>99</v>
       </c>
@@ -3216,7 +3261,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="17"/>
+      <c r="A100" s="15"/>
       <c r="B100" s="3" t="s">
         <v>100</v>
       </c>
@@ -3234,7 +3279,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="17"/>
+      <c r="A101" s="15"/>
       <c r="B101" s="3" t="s">
         <v>101</v>
       </c>
@@ -3252,7 +3297,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="17"/>
+      <c r="A102" s="15"/>
       <c r="B102" s="3" t="s">
         <v>102</v>
       </c>
@@ -3270,7 +3315,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="17"/>
+      <c r="A103" s="15"/>
       <c r="B103" s="3" t="s">
         <v>103</v>
       </c>
@@ -3288,7 +3333,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="17"/>
+      <c r="A104" s="15"/>
       <c r="B104" s="3" t="s">
         <v>104</v>
       </c>
@@ -3306,7 +3351,7 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="17"/>
+      <c r="A105" s="15"/>
       <c r="B105" s="3" t="s">
         <v>105</v>
       </c>
@@ -3324,7 +3369,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="17"/>
+      <c r="A106" s="15"/>
       <c r="B106" s="3" t="s">
         <v>106</v>
       </c>
@@ -3342,7 +3387,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="17"/>
+      <c r="A107" s="15"/>
       <c r="B107" s="3" t="s">
         <v>107</v>
       </c>
@@ -3360,7 +3405,7 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="17"/>
+      <c r="A108" s="15"/>
       <c r="B108" s="3" t="s">
         <v>108</v>
       </c>
@@ -3378,7 +3423,7 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="17"/>
+      <c r="A109" s="15"/>
       <c r="B109" s="3" t="s">
         <v>109</v>
       </c>
@@ -3396,7 +3441,7 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="17"/>
+      <c r="A110" s="15"/>
       <c r="B110" s="3" t="s">
         <v>110</v>
       </c>
@@ -3414,7 +3459,7 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="17"/>
+      <c r="A111" s="15"/>
       <c r="B111" s="3" t="s">
         <v>111</v>
       </c>
@@ -3432,7 +3477,7 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="17"/>
+      <c r="A112" s="15"/>
       <c r="B112" s="3" t="s">
         <v>112</v>
       </c>
@@ -3450,7 +3495,7 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="17"/>
+      <c r="A113" s="15"/>
       <c r="B113" s="3" t="s">
         <v>113</v>
       </c>
@@ -3468,7 +3513,7 @@
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="17"/>
+      <c r="A114" s="15"/>
       <c r="B114" s="3" t="s">
         <v>114</v>
       </c>
@@ -3486,7 +3531,7 @@
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="17"/>
+      <c r="A115" s="15"/>
       <c r="B115" s="3" t="s">
         <v>115</v>
       </c>
@@ -3504,7 +3549,7 @@
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="17"/>
+      <c r="A116" s="15"/>
       <c r="B116" s="3" t="s">
         <v>116</v>
       </c>
@@ -3522,7 +3567,7 @@
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="17"/>
+      <c r="A117" s="15"/>
       <c r="B117" s="3" t="s">
         <v>117</v>
       </c>
@@ -3540,7 +3585,7 @@
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="18"/>
+      <c r="A118" s="16"/>
       <c r="B118" s="3" t="s">
         <v>118</v>
       </c>
@@ -3551,14 +3596,14 @@
         <v>196</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="18"/>
+      <c r="A119" s="16"/>
       <c r="B119" s="3" t="s">
         <v>119</v>
       </c>
@@ -3569,14 +3614,14 @@
         <v>196</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="F119" s="4" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="18"/>
+      <c r="A120" s="16"/>
       <c r="B120" s="3" t="s">
         <v>120</v>
       </c>
@@ -3587,14 +3632,14 @@
         <v>196</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="18"/>
+      <c r="A121" s="16"/>
       <c r="B121" s="3" t="s">
         <v>121</v>
       </c>
@@ -3605,14 +3650,14 @@
         <v>196</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="18"/>
+      <c r="A122" s="16"/>
       <c r="B122" s="3" t="s">
         <v>122</v>
       </c>
@@ -3623,14 +3668,14 @@
         <v>196</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="F122" s="4" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="18"/>
+      <c r="A123" s="16"/>
       <c r="B123" s="3" t="s">
         <v>123</v>
       </c>
@@ -3641,14 +3686,14 @@
         <v>196</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="F123" s="4" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="18"/>
+      <c r="A124" s="16"/>
       <c r="B124" s="3" t="s">
         <v>211</v>
       </c>
@@ -3659,14 +3704,14 @@
         <v>196</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="18"/>
+      <c r="A125" s="16"/>
       <c r="B125" s="3" t="s">
         <v>124</v>
       </c>
@@ -3677,14 +3722,14 @@
         <v>196</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="F125" s="4" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="18"/>
+      <c r="A126" s="16"/>
       <c r="B126" s="3" t="s">
         <v>125</v>
       </c>
@@ -3695,14 +3740,14 @@
         <v>196</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="F126" s="4" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="18"/>
+      <c r="A127" s="16"/>
       <c r="B127" s="3" t="s">
         <v>126</v>
       </c>
@@ -3713,14 +3758,14 @@
         <v>196</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="F127" s="4" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="18"/>
+      <c r="A128" s="16"/>
       <c r="B128" s="3" t="s">
         <v>127</v>
       </c>
@@ -3731,14 +3776,14 @@
         <v>196</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="F128" s="4" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="18"/>
+      <c r="A129" s="16"/>
       <c r="B129" s="3" t="s">
         <v>128</v>
       </c>
@@ -3749,14 +3794,14 @@
         <v>196</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="F129" s="4" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" s="18"/>
+      <c r="A130" s="16"/>
       <c r="B130" s="3" t="s">
         <v>129</v>
       </c>
@@ -3767,14 +3812,14 @@
         <v>199</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F130" s="4" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" s="18"/>
+      <c r="A131" s="16"/>
       <c r="B131" s="3" t="s">
         <v>130</v>
       </c>
@@ -3785,14 +3830,14 @@
         <v>199</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F131" s="4" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" s="18"/>
+      <c r="A132" s="16"/>
       <c r="B132" s="3" t="s">
         <v>131</v>
       </c>
@@ -3803,14 +3848,14 @@
         <v>196</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="F132" s="4" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133" s="18"/>
+      <c r="A133" s="16"/>
       <c r="B133" s="3" t="s">
         <v>132</v>
       </c>
@@ -3821,32 +3866,32 @@
         <v>196</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="F133" s="4" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" s="18"/>
+      <c r="A134" s="16"/>
       <c r="B134" s="3" t="s">
         <v>133</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>185</v>
+        <v>230</v>
       </c>
       <c r="F134" s="4" t="s">
-        <v>185</v>
+        <v>230</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="19"/>
+      <c r="A135" s="17"/>
       <c r="B135" s="3" t="s">
         <v>134</v>
       </c>
@@ -3864,25 +3909,25 @@
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="19"/>
+      <c r="A136" s="17"/>
       <c r="B136" s="3" t="s">
         <v>135</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>22</v>
+        <v>185</v>
       </c>
       <c r="F136" s="4" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" s="19"/>
+      <c r="A137" s="17"/>
       <c r="B137" s="3" t="s">
         <v>136</v>
       </c>
@@ -3900,7 +3945,7 @@
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" s="19"/>
+      <c r="A138" s="17"/>
       <c r="B138" s="3" t="s">
         <v>137</v>
       </c>
@@ -3918,7 +3963,7 @@
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A139" s="19"/>
+      <c r="A139" s="17"/>
       <c r="B139" s="3" t="s">
         <v>138</v>
       </c>
@@ -3936,7 +3981,7 @@
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A140" s="19"/>
+      <c r="A140" s="17"/>
       <c r="B140" s="3" t="s">
         <v>139</v>
       </c>
@@ -3947,14 +3992,14 @@
         <v>196</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="F140" s="4" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A141" s="19"/>
+      <c r="A141" s="17"/>
       <c r="B141" s="3" t="s">
         <v>140</v>
       </c>
@@ -3965,14 +4010,14 @@
         <v>196</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="F141" s="4" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A142" s="19"/>
+      <c r="A142" s="17"/>
       <c r="B142" s="3" t="s">
         <v>141</v>
       </c>
@@ -3983,14 +4028,14 @@
         <v>196</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="F142" s="4" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A143" s="19"/>
+      <c r="A143" s="17"/>
       <c r="B143" s="3" t="s">
         <v>142</v>
       </c>
@@ -4001,14 +4046,14 @@
         <v>196</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="F143" s="4" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A144" s="19"/>
+      <c r="A144" s="17"/>
       <c r="B144" s="3" t="s">
         <v>143</v>
       </c>
@@ -4019,14 +4064,14 @@
         <v>196</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="F144" s="4" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" s="19"/>
+      <c r="A145" s="17"/>
       <c r="B145" s="3" t="s">
         <v>144</v>
       </c>
@@ -4037,14 +4082,14 @@
         <v>196</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="F145" s="4" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" s="19"/>
+      <c r="A146" s="17"/>
       <c r="B146" s="3" t="s">
         <v>145</v>
       </c>
@@ -4055,14 +4100,14 @@
         <v>196</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="F146" s="4" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A147" s="19"/>
+      <c r="A147" s="17"/>
       <c r="B147" s="3" t="s">
         <v>146</v>
       </c>
@@ -4073,14 +4118,14 @@
         <v>196</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="F147" s="4" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A148" s="20"/>
+      <c r="A148" s="18"/>
       <c r="B148" s="3" t="s">
         <v>147</v>
       </c>
@@ -4098,7 +4143,7 @@
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" s="20"/>
+      <c r="A149" s="18"/>
       <c r="B149" s="3" t="s">
         <v>148</v>
       </c>
@@ -4116,7 +4161,7 @@
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" s="20"/>
+      <c r="A150" s="18"/>
       <c r="B150" s="3" t="s">
         <v>149</v>
       </c>
@@ -4134,7 +4179,7 @@
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A151" s="20"/>
+      <c r="A151" s="18"/>
       <c r="B151" s="3" t="s">
         <v>150</v>
       </c>
@@ -4152,7 +4197,7 @@
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A152" s="20"/>
+      <c r="A152" s="18"/>
       <c r="B152" s="3" t="s">
         <v>151</v>
       </c>
@@ -4170,7 +4215,7 @@
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A153" s="20"/>
+      <c r="A153" s="18"/>
       <c r="B153" s="3" t="s">
         <v>152</v>
       </c>
@@ -4188,7 +4233,7 @@
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A154" s="20"/>
+      <c r="A154" s="18"/>
       <c r="B154" s="3" t="s">
         <v>153</v>
       </c>
@@ -4206,7 +4251,7 @@
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A155" s="20"/>
+      <c r="A155" s="18"/>
       <c r="B155" s="3" t="s">
         <v>154</v>
       </c>
@@ -4224,7 +4269,7 @@
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A156" s="20"/>
+      <c r="A156" s="18"/>
       <c r="B156" s="3" t="s">
         <v>155</v>
       </c>
@@ -4242,7 +4287,7 @@
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A157" s="20"/>
+      <c r="A157" s="18"/>
       <c r="B157" s="3" t="s">
         <v>156</v>
       </c>
@@ -4260,7 +4305,7 @@
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A158" s="20"/>
+      <c r="A158" s="18"/>
       <c r="B158" s="3" t="s">
         <v>157</v>
       </c>
@@ -4278,7 +4323,7 @@
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A159" s="20"/>
+      <c r="A159" s="18"/>
       <c r="B159" s="3" t="s">
         <v>158</v>
       </c>
@@ -4296,7 +4341,7 @@
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A160" s="20"/>
+      <c r="A160" s="18"/>
       <c r="B160" s="3" t="s">
         <v>159</v>
       </c>
@@ -4314,7 +4359,7 @@
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A161" s="20"/>
+      <c r="A161" s="18"/>
       <c r="B161" s="3" t="s">
         <v>160</v>
       </c>
@@ -4332,7 +4377,7 @@
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A162" s="20"/>
+      <c r="A162" s="18"/>
       <c r="B162" s="3" t="s">
         <v>161</v>
       </c>
@@ -4350,7 +4395,7 @@
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A163" s="20"/>
+      <c r="A163" s="18"/>
       <c r="B163" s="3" t="s">
         <v>162</v>
       </c>
@@ -4368,43 +4413,43 @@
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A164" s="20"/>
+      <c r="A164" s="18"/>
       <c r="B164" s="3" t="s">
         <v>163</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E164" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F164" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="F164" s="4" t="s">
-        <v>254</v>
-      </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A165" s="20"/>
+      <c r="A165" s="18"/>
       <c r="B165" s="3" t="s">
         <v>164</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>253</v>
+        <v>185</v>
       </c>
       <c r="F165" s="4" t="s">
-        <v>255</v>
+        <v>185</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A166" s="21"/>
+      <c r="A166" s="19"/>
       <c r="B166" s="3" t="s">
         <v>165</v>
       </c>
@@ -4412,17 +4457,17 @@
         <v>200</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="F166" s="4" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A167" s="21"/>
+      <c r="A167" s="19"/>
       <c r="B167" s="3" t="s">
         <v>166</v>
       </c>
@@ -4430,17 +4475,17 @@
         <v>200</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="F167" s="4" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A168" s="21"/>
+      <c r="A168" s="19"/>
       <c r="B168" s="3" t="s">
         <v>167</v>
       </c>
@@ -4448,17 +4493,17 @@
         <v>200</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E168" s="2" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="F168" s="4" t="s">
-        <v>251</v>
+        <v>293</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A169" s="21"/>
+      <c r="A169" s="19"/>
       <c r="B169" s="3" t="s">
         <v>168</v>
       </c>
@@ -4466,17 +4511,17 @@
         <v>200</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E169" s="2" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="F169" s="4" t="s">
-        <v>251</v>
+        <v>292</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A170" s="21"/>
+      <c r="A170" s="19"/>
       <c r="B170" s="3" t="s">
         <v>169</v>
       </c>
@@ -4484,17 +4529,17 @@
         <v>200</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="F170" s="4" t="s">
-        <v>251</v>
+        <v>291</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A171" s="21"/>
+      <c r="A171" s="19"/>
       <c r="B171" s="3" t="s">
         <v>170</v>
       </c>
@@ -4502,17 +4547,17 @@
         <v>200</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="F171" s="4" t="s">
-        <v>251</v>
+        <v>290</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A172" s="21"/>
+      <c r="A172" s="19"/>
       <c r="B172" s="3" t="s">
         <v>171</v>
       </c>
@@ -4520,17 +4565,17 @@
         <v>200</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E172" s="2" t="s">
-        <v>250</v>
+        <v>266</v>
       </c>
       <c r="F172" s="4" t="s">
-        <v>251</v>
+        <v>289</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A173" s="21"/>
+      <c r="A173" s="19"/>
       <c r="B173" s="3" t="s">
         <v>172</v>
       </c>
@@ -4538,17 +4583,17 @@
         <v>200</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E173" s="2" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="F173" s="4" t="s">
-        <v>251</v>
+        <v>288</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A174" s="21"/>
+      <c r="A174" s="19"/>
       <c r="B174" s="3" t="s">
         <v>173</v>
       </c>
@@ -4556,17 +4601,17 @@
         <v>200</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E174" s="2" t="s">
-        <v>250</v>
+        <v>268</v>
       </c>
       <c r="F174" s="4" t="s">
-        <v>251</v>
+        <v>269</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A175" s="21"/>
+      <c r="A175" s="19"/>
       <c r="B175" s="3" t="s">
         <v>174</v>
       </c>
@@ -4574,17 +4619,17 @@
         <v>200</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E175" s="2" t="s">
-        <v>250</v>
+        <v>272</v>
       </c>
       <c r="F175" s="4" t="s">
-        <v>251</v>
+        <v>287</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A176" s="21"/>
+      <c r="A176" s="19"/>
       <c r="B176" s="3" t="s">
         <v>175</v>
       </c>
@@ -4592,17 +4637,17 @@
         <v>200</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F176" s="4" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A177" s="21"/>
+      <c r="A177" s="19"/>
       <c r="B177" s="3" t="s">
         <v>176</v>
       </c>
@@ -4610,125 +4655,125 @@
         <v>200</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F177" s="4" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A178" s="21"/>
+      <c r="A178" s="19"/>
       <c r="B178" s="3" t="s">
         <v>177</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>185</v>
+        <v>275</v>
       </c>
       <c r="F178" s="4" t="s">
-        <v>185</v>
+        <v>284</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A179" s="21"/>
+      <c r="A179" s="19"/>
       <c r="B179" s="3" t="s">
         <v>178</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>185</v>
+        <v>276</v>
       </c>
       <c r="F179" s="4" t="s">
-        <v>185</v>
+        <v>283</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A180" s="21"/>
+      <c r="A180" s="19"/>
       <c r="B180" s="3" t="s">
         <v>179</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>185</v>
+        <v>277</v>
       </c>
       <c r="F180" s="4" t="s">
-        <v>185</v>
+        <v>282</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A181" s="21"/>
+      <c r="A181" s="19"/>
       <c r="B181" s="3" t="s">
         <v>180</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>185</v>
+        <v>278</v>
       </c>
       <c r="F181" s="4" t="s">
-        <v>185</v>
+        <v>281</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A182" s="21"/>
+      <c r="A182" s="19"/>
       <c r="B182" s="3" t="s">
         <v>181</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="E182" s="2" t="s">
-        <v>185</v>
+        <v>279</v>
       </c>
       <c r="F182" s="4" t="s">
-        <v>185</v>
+        <v>280</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A183" s="21"/>
+      <c r="A183" s="19"/>
       <c r="B183" s="3" t="s">
         <v>182</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>185</v>
+        <v>270</v>
       </c>
       <c r="F183" s="4" t="s">
-        <v>185</v>
+        <v>271</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A184" s="21"/>
+      <c r="A184" s="19"/>
       <c r="B184" s="3" t="s">
         <v>183</v>
       </c>
@@ -4746,7 +4791,7 @@
       </c>
     </row>
     <row r="185" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A185" s="21"/>
+      <c r="A185" s="19"/>
       <c r="B185" s="5" t="s">
         <v>184</v>
       </c>

</xml_diff>

<commit_message>
Added components library to Altium and placed parts on schematic.
</commit_message>
<xml_diff>
--- a/Documentation/cyclone-iii-pinout.xlsx
+++ b/Documentation/cyclone-iii-pinout.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="295">
   <si>
     <t>Pin</t>
   </si>
@@ -901,6 +901,9 @@
   </si>
   <si>
     <t>User-selectable port 10</t>
+  </si>
+  <si>
+    <t>Extra Switch Input</t>
   </si>
 </sst>
 </file>
@@ -1539,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H168" sqref="H168"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L173" sqref="L173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2618,16 +2621,16 @@
         <v>65</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>185</v>
+        <v>230</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>185</v>
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2996,16 +2999,16 @@
         <v>85</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>185</v>
+        <v>294</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>185</v>
+        <v>294</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -3914,16 +3917,16 @@
         <v>135</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>185</v>
+        <v>294</v>
       </c>
       <c r="F136" s="4" t="s">
-        <v>185</v>
+        <v>294</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -3932,16 +3935,16 @@
         <v>136</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>185</v>
+        <v>294</v>
       </c>
       <c r="F137" s="4" t="s">
-        <v>185</v>
+        <v>294</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -3950,16 +3953,16 @@
         <v>137</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>185</v>
+        <v>294</v>
       </c>
       <c r="F138" s="4" t="s">
-        <v>185</v>
+        <v>294</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
@@ -4778,16 +4781,16 @@
         <v>183</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="E184" s="2" t="s">
-        <v>185</v>
+        <v>294</v>
       </c>
       <c r="F184" s="4" t="s">
-        <v>185</v>
+        <v>294</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4796,16 +4799,16 @@
         <v>184</v>
       </c>
       <c r="C185" s="6" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D185" s="6" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="E185" s="6" t="s">
-        <v>185</v>
+        <v>294</v>
       </c>
       <c r="F185" s="7" t="s">
-        <v>185</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>